<commit_message>
Finished My Excel Chart
Updated Quantity from Alireza's calculation
</commit_message>
<xml_diff>
--- a/Capstone Project/Monika/Costs PerV4.xlsx
+++ b/Capstone Project/Monika/Costs PerV4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mszuc\Desktop\Capstone-Project-Data-Modeling-and-PowerBI\Capstone Project\Monika\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F27A6DD-468D-4B61-9A95-4C0D71BDB9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC01A50-D4A3-49D9-9E58-80C4E4974711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{ED117939-1D2E-4498-B130-96B64592D033}"/>
   </bookViews>
@@ -148,13 +148,13 @@
     <t>% of Repairs needed Extreme</t>
   </si>
   <si>
-    <t>2015 to 2019 Repair Sales in BC</t>
-  </si>
-  <si>
     <t>Changes the numbers from Alireza's report based on the 7 cards</t>
   </si>
   <si>
     <t>The red numbers are Taralynns totals but alireza needs to calculate per car which needs to be changed</t>
+  </si>
+  <si>
+    <t>2015 to 2019 Repair Sales in Canada</t>
   </si>
 </sst>
 </file>
@@ -223,7 +223,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -656,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6105DF2C-7430-48BF-A45E-C623D48AA4A1}">
   <dimension ref="A2:CK66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -674,7 +673,13 @@
     <col min="12" max="12" width="19.1328125" customWidth="1"/>
     <col min="13" max="13" width="21.6640625" customWidth="1"/>
     <col min="14" max="14" width="18.33203125" customWidth="1"/>
-    <col min="15" max="21" width="12.73046875" customWidth="1"/>
+    <col min="15" max="15" width="16.9296875" customWidth="1"/>
+    <col min="16" max="16" width="18.265625" customWidth="1"/>
+    <col min="17" max="17" width="16.53125" customWidth="1"/>
+    <col min="18" max="18" width="18.06640625" customWidth="1"/>
+    <col min="19" max="19" width="19.19921875" customWidth="1"/>
+    <col min="20" max="20" width="18.9296875" customWidth="1"/>
+    <col min="21" max="21" width="12.73046875" customWidth="1"/>
     <col min="22" max="22" width="18.3984375" customWidth="1"/>
     <col min="23" max="23" width="21.33203125" customWidth="1"/>
     <col min="24" max="24" width="19.73046875" customWidth="1"/>
@@ -693,7 +698,7 @@
   <sheetData>
     <row r="2" spans="1:24" ht="38.25" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4"/>
     </row>
@@ -1124,7 +1129,7 @@
         <v>2019</v>
       </c>
       <c r="B17" s="7">
-        <v>25</v>
+        <v>45098</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>17</v>
@@ -1135,49 +1140,49 @@
       <c r="G17" s="29"/>
       <c r="H17" s="29">
         <f>$M6 * (B17*B11)</f>
-        <v>1500</v>
+        <v>2705880</v>
       </c>
       <c r="I17" s="24">
         <f>SUM(D17:H17)</f>
-        <v>1500</v>
+        <v>2705880</v>
       </c>
       <c r="J17" s="29"/>
       <c r="K17" s="5">
         <f>$I6 * (B17*B12)</f>
-        <v>10000</v>
+        <v>18039200</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="24">
         <f t="shared" ref="M17:M23" si="0">SUM(J17:L17)</f>
-        <v>10000</v>
+        <v>18039200</v>
       </c>
       <c r="N17" s="5">
         <f>$A6 * (B17*B13)</f>
-        <v>6000</v>
+        <v>10823520</v>
       </c>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5">
         <f>$G6 * (B17*B13)</f>
-        <v>11000</v>
+        <v>19843120</v>
       </c>
       <c r="R17" s="5">
         <f>$H6 * (B17*B13)</f>
-        <v>3000</v>
+        <v>5411760</v>
       </c>
       <c r="S17" s="24">
         <f t="shared" ref="S17:S23" si="1">SUM(N17:R17)</f>
-        <v>20000</v>
+        <v>36078400</v>
       </c>
       <c r="T17" s="25">
         <f>SUM(I17+M17)</f>
-        <v>11500</v>
+        <v>20745080</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A18" s="17"/>
       <c r="B18" s="7">
-        <v>20</v>
+        <v>38970</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
@@ -1185,46 +1190,46 @@
       <c r="D18" s="29"/>
       <c r="E18" s="29">
         <f>$C6 * (B18*B11)</f>
-        <v>2400</v>
+        <v>4676400</v>
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
       <c r="H18" s="5"/>
       <c r="I18" s="24">
         <f t="shared" ref="I18:I39" si="2">SUM(D18:H18)</f>
-        <v>2400</v>
+        <v>4676400</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5">
         <f>$I6 * (B18*B12)</f>
-        <v>8000</v>
+        <v>15588000</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="24">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>15588000</v>
       </c>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5">
         <f>$F6 * (B18*B13)</f>
-        <v>6080</v>
+        <v>11846880</v>
       </c>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
       <c r="S18" s="24">
         <f t="shared" si="1"/>
-        <v>6080</v>
+        <v>11846880</v>
       </c>
       <c r="T18" s="25">
         <f t="shared" ref="T18:T22" si="3">SUM(I18+M18)</f>
-        <v>10400</v>
+        <v>20264400</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A19" s="17"/>
       <c r="B19" s="7">
-        <v>18</v>
+        <v>35825</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>19</v>
@@ -1234,47 +1239,47 @@
       <c r="F19" s="29"/>
       <c r="G19" s="29">
         <f>$L6 * (B19*B11)</f>
-        <v>2160</v>
+        <v>4299000</v>
       </c>
       <c r="H19" s="29"/>
       <c r="I19" s="24">
         <f t="shared" si="2"/>
-        <v>2160</v>
+        <v>4299000</v>
       </c>
       <c r="J19" s="5">
         <f>$D6 * (B19*B12)</f>
-        <v>720</v>
+        <v>1433000</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="24">
         <f t="shared" si="0"/>
-        <v>720</v>
+        <v>1433000</v>
       </c>
       <c r="N19" s="5"/>
       <c r="O19" s="5">
         <f>$E6 * (B19*B13)</f>
-        <v>6480</v>
+        <v>12897000</v>
       </c>
       <c r="P19" s="5"/>
       <c r="Q19" s="5">
         <f>$G6 * (B19*B13)</f>
-        <v>7920</v>
+        <v>15763000</v>
       </c>
       <c r="R19" s="5"/>
       <c r="S19" s="24">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>28660000</v>
       </c>
       <c r="T19" s="25">
         <f t="shared" si="3"/>
-        <v>2880</v>
+        <v>5732000</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A20" s="17"/>
       <c r="B20" s="7">
-        <v>19</v>
+        <v>24213</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>20</v>
@@ -1282,117 +1287,117 @@
       <c r="D20" s="29"/>
       <c r="E20" s="29">
         <f>$C6 * (B20*B11)</f>
-        <v>2280</v>
+        <v>2905560</v>
       </c>
       <c r="F20" s="29">
         <f>$K6 * (B20*B11)</f>
-        <v>5016</v>
+        <v>6392232</v>
       </c>
       <c r="G20" s="29"/>
       <c r="H20" s="29">
         <f>$M6 * (B20*B11)</f>
-        <v>1140</v>
+        <v>1452780</v>
       </c>
       <c r="I20" s="24">
         <f t="shared" si="2"/>
-        <v>8436</v>
+        <v>10750572</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5">
         <f>$I6 * (B20*B12)</f>
-        <v>7600</v>
+        <v>9685200</v>
       </c>
       <c r="L20" s="5">
         <f>$J6 * (B20*B12)</f>
-        <v>2565</v>
+        <v>3268755</v>
       </c>
       <c r="M20" s="24">
         <f t="shared" si="0"/>
-        <v>10165</v>
+        <v>12953955</v>
       </c>
       <c r="N20" s="5"/>
       <c r="O20" s="5">
         <f>$E6 * (B20*B13)</f>
-        <v>6840.0000000000009</v>
+        <v>8716680</v>
       </c>
       <c r="P20" s="5">
         <f>$F6 * (B20*B13)</f>
-        <v>5776</v>
+        <v>7360752.0000000009</v>
       </c>
       <c r="Q20" s="5"/>
       <c r="R20" s="5">
         <f>$H6 * (B20*B13)</f>
-        <v>2280</v>
+        <v>2905560</v>
       </c>
       <c r="S20" s="24">
         <f t="shared" si="1"/>
-        <v>14896</v>
+        <v>18982992</v>
       </c>
       <c r="T20" s="25">
         <f t="shared" si="3"/>
-        <v>18601</v>
+        <v>23704527</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A21" s="17"/>
       <c r="B21" s="7">
-        <v>21</v>
+        <v>26345</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="29">
         <f>$B6 * (B21*B11)</f>
-        <v>15120</v>
+        <v>18968400</v>
       </c>
       <c r="E21" s="29">
         <f>$C6 * (B21*B11)</f>
-        <v>2520</v>
+        <v>3161400</v>
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
       <c r="H21" s="29">
         <f>$M6 * (B21*B11)</f>
-        <v>1260</v>
+        <v>1580700</v>
       </c>
       <c r="I21" s="24">
         <f t="shared" si="2"/>
-        <v>18900</v>
+        <v>23710500</v>
       </c>
       <c r="J21" s="5">
         <f>$D6 * (B21*B12)</f>
-        <v>840</v>
+        <v>1053800</v>
       </c>
       <c r="K21" s="5">
         <f>$I6 * (B21*B12)</f>
-        <v>8400</v>
+        <v>10538000</v>
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="24">
         <f t="shared" si="0"/>
-        <v>9240</v>
+        <v>11591800</v>
       </c>
       <c r="N21" s="5"/>
       <c r="O21" s="5">
         <f>$E6 * (B21*B13)</f>
-        <v>7560</v>
+        <v>9484200</v>
       </c>
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
       <c r="S21" s="24">
         <f t="shared" si="1"/>
-        <v>7560</v>
+        <v>9484200</v>
       </c>
       <c r="T21" s="25">
         <f t="shared" si="3"/>
-        <v>28140</v>
+        <v>35302300</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A22" s="17"/>
       <c r="B22" s="7">
-        <v>22</v>
+        <v>25968</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>22</v>
@@ -1402,29 +1407,29 @@
       <c r="F22" s="29"/>
       <c r="G22" s="29">
         <f>$L6 * (B22*B11)</f>
-        <v>2640</v>
+        <v>3116160</v>
       </c>
       <c r="H22" s="29"/>
       <c r="I22" s="24">
         <f t="shared" si="2"/>
-        <v>2640</v>
+        <v>3116160</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5">
         <f>$I6 * (B22*B12)</f>
-        <v>8800</v>
+        <v>10387200</v>
       </c>
       <c r="L22" s="5">
         <f>$J6 * (B22*B12)</f>
-        <v>2970</v>
+        <v>3505680</v>
       </c>
       <c r="M22" s="24">
         <f t="shared" si="0"/>
-        <v>11770</v>
+        <v>13892880</v>
       </c>
       <c r="N22" s="5">
         <f>$A6 * (B22*B13)</f>
-        <v>5280</v>
+        <v>6232320</v>
       </c>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
@@ -1432,17 +1437,17 @@
       <c r="R22" s="5"/>
       <c r="S22" s="24">
         <f t="shared" si="1"/>
-        <v>5280</v>
+        <v>6232320</v>
       </c>
       <c r="T22" s="25">
         <f t="shared" si="3"/>
-        <v>14410</v>
+        <v>17009040</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A23" s="17"/>
       <c r="B23" s="7">
-        <v>20</v>
+        <v>28322</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>23</v>
@@ -1450,49 +1455,49 @@
       <c r="D23" s="29"/>
       <c r="E23" s="29">
         <f>$C6 * (B23*B11)</f>
-        <v>2400</v>
+        <v>3398640</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="29"/>
       <c r="H23" s="29">
         <f>$M6 * (B23*B11)</f>
-        <v>1200</v>
+        <v>1699320</v>
       </c>
       <c r="I23" s="24">
         <f>SUM(D23:H23)</f>
-        <v>3600</v>
+        <v>5097960</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5">
         <f>$I6 * (B23*B12)</f>
-        <v>8000</v>
+        <v>11328800</v>
       </c>
       <c r="L23" s="5"/>
       <c r="M23" s="24">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>11328800</v>
       </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5">
         <f>$E6 * (B23*B13)</f>
-        <v>7200</v>
+        <v>10195920.000000002</v>
       </c>
       <c r="P23" s="5">
         <f>$F6 * (B23*B13)</f>
-        <v>6080</v>
+        <v>8609888</v>
       </c>
       <c r="Q23" s="5"/>
       <c r="R23" s="5">
         <f>$H6 * (B23*B13)</f>
-        <v>2400</v>
+        <v>3398640.0000000005</v>
       </c>
       <c r="S23" s="24">
         <f t="shared" si="1"/>
-        <v>15680</v>
+        <v>22204448</v>
       </c>
       <c r="T23" s="25">
         <f>SUM(I23+M23)</f>
-        <v>11600</v>
+        <v>16426760</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.45">
@@ -1500,76 +1505,77 @@
         <v>30</v>
       </c>
       <c r="B24" s="31">
-        <v>237091</v>
+        <f>SUM(B17:B23)</f>
+        <v>224741</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="24">
         <f t="shared" ref="D24:I24" si="4">SUM(D17:D23)</f>
-        <v>15120</v>
+        <v>18968400</v>
       </c>
       <c r="E24" s="24">
         <f t="shared" si="4"/>
-        <v>9600</v>
+        <v>14142000</v>
       </c>
       <c r="F24" s="24">
         <f t="shared" si="4"/>
-        <v>5016</v>
+        <v>6392232</v>
       </c>
       <c r="G24" s="24">
         <f t="shared" si="4"/>
-        <v>4800</v>
+        <v>7415160</v>
       </c>
       <c r="H24" s="24">
         <f t="shared" si="4"/>
-        <v>5100</v>
+        <v>7438680</v>
       </c>
       <c r="I24" s="24">
         <f t="shared" si="4"/>
-        <v>39636</v>
+        <v>54356472</v>
       </c>
       <c r="J24" s="24">
         <f t="shared" ref="J24:R24" si="5">SUM(J17:J23)</f>
-        <v>1560</v>
+        <v>2486800</v>
       </c>
       <c r="K24" s="24">
         <f t="shared" si="5"/>
-        <v>50800</v>
+        <v>75566400</v>
       </c>
       <c r="L24" s="24">
         <f t="shared" si="5"/>
-        <v>5535</v>
+        <v>6774435</v>
       </c>
       <c r="M24" s="24">
         <f>SUM(M17:M23)</f>
-        <v>57895</v>
+        <v>84827635</v>
       </c>
       <c r="N24" s="24">
         <f t="shared" si="5"/>
-        <v>11280</v>
+        <v>17055840</v>
       </c>
       <c r="O24" s="24">
         <f t="shared" si="5"/>
-        <v>28080</v>
+        <v>41293800</v>
       </c>
       <c r="P24" s="24">
         <f t="shared" si="5"/>
-        <v>17936</v>
+        <v>27817520</v>
       </c>
       <c r="Q24" s="24">
         <f t="shared" si="5"/>
-        <v>18920</v>
+        <v>35606120</v>
       </c>
       <c r="R24" s="24">
         <f t="shared" si="5"/>
-        <v>7680</v>
+        <v>11715960</v>
       </c>
       <c r="S24" s="24">
         <f>SUM(S17:S23)</f>
-        <v>83896</v>
+        <v>133489240</v>
       </c>
       <c r="T24" s="25">
         <f>SUM(I24+M24)</f>
-        <v>97531</v>
+        <v>139184107</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.45">
@@ -1577,7 +1583,7 @@
         <v>2018</v>
       </c>
       <c r="B25" s="7">
-        <v>31</v>
+        <v>44274</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>17</v>
@@ -1588,21 +1594,21 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5">
         <f>$M6 * (B25*B11)</f>
-        <v>1859.9999999999998</v>
+        <v>2656440</v>
       </c>
       <c r="I25" s="24">
         <f t="shared" si="2"/>
-        <v>1859.9999999999998</v>
+        <v>2656440</v>
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5">
         <f>$I6 * (B25*B12)</f>
-        <v>12400</v>
+        <v>17709600</v>
       </c>
       <c r="L25" s="5"/>
       <c r="M25" s="24">
         <f t="shared" ref="M25:M39" si="6">SUM(J25:L25)</f>
-        <v>12400</v>
+        <v>17709600</v>
       </c>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
@@ -1610,21 +1616,21 @@
       <c r="Q25" s="5"/>
       <c r="R25" s="5">
         <f>$H6 * (B25*B13)</f>
-        <v>3720</v>
+        <v>5312880.0000000009</v>
       </c>
       <c r="S25" s="24">
         <f t="shared" ref="S25:S39" si="7">SUM(N25:R25)</f>
-        <v>3720</v>
+        <v>5312880.0000000009</v>
       </c>
       <c r="T25" s="25">
         <f>SUM(I25+M25+S25)</f>
-        <v>17980</v>
+        <v>25678920</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A26" s="17"/>
       <c r="B26" s="7">
-        <v>17</v>
+        <v>38253</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>18</v>
@@ -1632,111 +1638,111 @@
       <c r="D26" s="5"/>
       <c r="E26" s="5">
         <f>$C6 * (B26*B11)</f>
-        <v>2039.9999999999998</v>
+        <v>4590360</v>
       </c>
       <c r="F26" s="5">
         <f>$K6 * (B26*B11)</f>
-        <v>4488</v>
+        <v>10098792</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5">
         <f>$M6 * (B26*B11)</f>
-        <v>1019.9999999999999</v>
+        <v>2295180</v>
       </c>
       <c r="I26" s="24">
         <f t="shared" si="2"/>
-        <v>7548</v>
+        <v>16984332</v>
       </c>
       <c r="J26" s="5">
         <f>$D6 * (B26*B12)</f>
-        <v>680</v>
+        <v>1530120</v>
       </c>
       <c r="K26" s="5">
         <f>$I6 * (B26*B12)</f>
-        <v>6800</v>
+        <v>15301200</v>
       </c>
       <c r="L26" s="5"/>
       <c r="M26" s="24">
         <f t="shared" si="6"/>
-        <v>7480</v>
+        <v>16831320</v>
       </c>
       <c r="N26" s="5"/>
       <c r="O26" s="5">
         <f>$E6 * (B26*B13)</f>
-        <v>6120.0000000000009</v>
+        <v>13771080</v>
       </c>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
       <c r="S26" s="24">
         <f t="shared" si="7"/>
-        <v>6120.0000000000009</v>
+        <v>13771080</v>
       </c>
       <c r="T26" s="25">
         <f t="shared" ref="T26:T40" si="8">SUM(I26+M26+S26)</f>
-        <v>21148</v>
+        <v>47586732</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A27" s="17"/>
       <c r="B27" s="7">
-        <v>24</v>
+        <v>35347</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D27" s="5">
         <f>$B6 * (B27*B11)</f>
-        <v>17280</v>
+        <v>25449840</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5">
         <f>$M6 * (B27*B11)</f>
-        <v>1439.9999999999998</v>
+        <v>2120820</v>
       </c>
       <c r="I27" s="24">
         <f t="shared" si="2"/>
-        <v>18720</v>
+        <v>27570660</v>
       </c>
       <c r="J27" s="5">
         <f>$D6 * (B27*B12)</f>
-        <v>960</v>
+        <v>1413880</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5">
         <f>$J6 * (B27*B12)</f>
-        <v>3240</v>
+        <v>4771845</v>
       </c>
       <c r="M27" s="24">
         <f t="shared" si="6"/>
-        <v>4200</v>
+        <v>6185725</v>
       </c>
       <c r="N27" s="5">
         <f>$A6 * (B27*B13)</f>
-        <v>5760.0000000000009</v>
+        <v>8483280</v>
       </c>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="5">
         <f>$H6 * (B27*B13)</f>
-        <v>2880.0000000000005</v>
+        <v>4241640</v>
       </c>
       <c r="S27" s="24">
         <f t="shared" si="7"/>
-        <v>8640.0000000000018</v>
+        <v>12724920</v>
       </c>
       <c r="T27" s="25">
         <f t="shared" si="8"/>
-        <v>31560</v>
+        <v>46481305</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A28" s="17"/>
       <c r="B28" s="7">
-        <v>21</v>
+        <v>23254</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>20</v>
@@ -1745,54 +1751,54 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5">
         <f>$K6 * (B28*B11)</f>
-        <v>5544</v>
+        <v>6139056</v>
       </c>
       <c r="G28" s="5">
         <f>$L6 * (B28*B11)</f>
-        <v>2520</v>
+        <v>2790480</v>
       </c>
       <c r="H28" s="5">
         <f>$M6 * (B28*B11)</f>
-        <v>1260</v>
+        <v>1395240</v>
       </c>
       <c r="I28" s="24">
         <f t="shared" si="2"/>
-        <v>9324</v>
+        <v>10324776</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5">
         <f>$I6 * (B27*B12)</f>
-        <v>9600</v>
+        <v>14138800</v>
       </c>
       <c r="L28" s="5"/>
       <c r="M28" s="24">
         <f t="shared" si="6"/>
-        <v>9600</v>
+        <v>14138800</v>
       </c>
       <c r="N28" s="5"/>
       <c r="O28" s="5">
         <f>$E6 * (B28*B13)</f>
-        <v>7560</v>
+        <v>8371440</v>
       </c>
       <c r="P28" s="5">
         <f>$F6 * (B28*B13)</f>
-        <v>6384</v>
+        <v>7069216</v>
       </c>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
       <c r="S28" s="24">
         <f t="shared" si="7"/>
-        <v>13944</v>
+        <v>15440656</v>
       </c>
       <c r="T28" s="25">
         <f t="shared" si="8"/>
-        <v>32868</v>
+        <v>39904232</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A29" s="17"/>
       <c r="B29" s="7">
-        <v>26</v>
+        <v>25421</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>21</v>
@@ -1800,52 +1806,52 @@
       <c r="D29" s="5"/>
       <c r="E29" s="5">
         <f>$C6 * (B29*B11)</f>
-        <v>3120</v>
+        <v>3050519.9999999995</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5">
         <f>$M6 * (B29*B11)</f>
-        <v>1560</v>
+        <v>1525259.9999999998</v>
       </c>
       <c r="I29" s="24">
         <f t="shared" si="2"/>
-        <v>4680</v>
+        <v>4575779.9999999991</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5">
         <f>$I6 * (B29*B12)</f>
-        <v>10400</v>
+        <v>10168400</v>
       </c>
       <c r="L29" s="5"/>
       <c r="M29" s="24">
         <f t="shared" si="6"/>
-        <v>10400</v>
+        <v>10168400</v>
       </c>
       <c r="N29" s="5"/>
       <c r="O29" s="5">
         <f>$E6 * (B29*B13)</f>
-        <v>9360</v>
+        <v>9151560.0000000019</v>
       </c>
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="5">
         <f>$H6 * (B29*B13)</f>
-        <v>3120</v>
+        <v>3050520.0000000005</v>
       </c>
       <c r="S29" s="24">
         <f t="shared" si="7"/>
-        <v>12480</v>
+        <v>12202080.000000002</v>
       </c>
       <c r="T29" s="25">
         <f t="shared" si="8"/>
-        <v>27560</v>
+        <v>26946260</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A30" s="17"/>
       <c r="B30" s="7">
-        <v>17</v>
+        <v>25180</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>22</v>
@@ -1855,94 +1861,94 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5">
         <f>$L6 * (B30*B11)</f>
-        <v>2039.9999999999998</v>
+        <v>3021600</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="24">
         <f t="shared" si="2"/>
-        <v>2039.9999999999998</v>
+        <v>3021600</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5">
         <f>$J6 * (B30*B12)</f>
-        <v>2295</v>
+        <v>3399300</v>
       </c>
       <c r="M30" s="24">
         <f t="shared" si="6"/>
-        <v>2295</v>
+        <v>3399300</v>
       </c>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="5">
         <f>$G6 * (B30*B13)</f>
-        <v>7480.0000000000009</v>
+        <v>11079200</v>
       </c>
       <c r="R30" s="5"/>
       <c r="S30" s="24">
         <f t="shared" si="7"/>
-        <v>7480.0000000000009</v>
+        <v>11079200</v>
       </c>
       <c r="T30" s="25">
         <f t="shared" si="8"/>
-        <v>11815</v>
+        <v>17500100</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A31" s="17"/>
       <c r="B31" s="7">
-        <v>12</v>
+        <v>27256</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D31" s="5">
         <f>$B6 * B31</f>
-        <v>14400</v>
+        <v>32707200</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5">
         <f>$M6 * (B31*B11)</f>
-        <v>719.99999999999989</v>
+        <v>1635359.9999999998</v>
       </c>
       <c r="I31" s="24">
         <f t="shared" si="2"/>
-        <v>15120</v>
+        <v>34342560</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5">
         <f>$J6 * (B31*B12)</f>
-        <v>1620</v>
+        <v>3679560</v>
       </c>
       <c r="M31" s="24">
         <f t="shared" si="6"/>
-        <v>1620</v>
+        <v>3679560</v>
       </c>
       <c r="N31" s="5">
         <f>$A6 * (B31*B13)</f>
-        <v>2880.0000000000005</v>
+        <v>6541440.0000000009</v>
       </c>
       <c r="O31" s="5"/>
       <c r="P31" s="5">
         <f>$F6 * (B31*B13)</f>
-        <v>3648.0000000000005</v>
+        <v>8285824.0000000009</v>
       </c>
       <c r="Q31" s="5"/>
       <c r="R31" s="5">
         <f>$H6 * (B31*B13)</f>
-        <v>1440.0000000000002</v>
+        <v>3270720.0000000005</v>
       </c>
       <c r="S31" s="24">
         <f t="shared" si="7"/>
-        <v>7968.0000000000009</v>
+        <v>18097984.000000004</v>
       </c>
       <c r="T31" s="25">
         <f t="shared" si="8"/>
-        <v>24708</v>
+        <v>56120104</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.45">
@@ -1950,76 +1956,77 @@
         <v>32</v>
       </c>
       <c r="B32" s="31">
-        <v>231646</v>
+        <f>SUM(B25:B31)</f>
+        <v>218985</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="24">
         <f>SUM(D25:D31)</f>
-        <v>31680</v>
+        <v>58157040</v>
       </c>
       <c r="E32" s="24">
         <f t="shared" ref="E32:H32" si="9">SUM(E25:E31)</f>
-        <v>5160</v>
+        <v>7640880</v>
       </c>
       <c r="F32" s="24">
         <f t="shared" si="9"/>
-        <v>10032</v>
+        <v>16237848</v>
       </c>
       <c r="G32" s="24">
         <f t="shared" si="9"/>
-        <v>4560</v>
+        <v>5812080</v>
       </c>
       <c r="H32" s="24">
         <f t="shared" si="9"/>
-        <v>7859.9999999999991</v>
+        <v>11628300</v>
       </c>
       <c r="I32" s="24">
         <f t="shared" ref="I32:O32" si="10">SUM(I25:I31)</f>
-        <v>59292</v>
+        <v>99476148</v>
       </c>
       <c r="J32" s="24">
         <f t="shared" si="10"/>
-        <v>1640</v>
+        <v>2944000</v>
       </c>
       <c r="K32" s="24">
         <f t="shared" si="10"/>
-        <v>39200</v>
+        <v>57318000</v>
       </c>
       <c r="L32" s="24">
         <f t="shared" si="10"/>
-        <v>7155</v>
+        <v>11850705</v>
       </c>
       <c r="M32" s="24">
         <f t="shared" si="10"/>
-        <v>47995</v>
+        <v>72112705</v>
       </c>
       <c r="N32" s="24">
         <f t="shared" si="10"/>
-        <v>8640.0000000000018</v>
+        <v>15024720</v>
       </c>
       <c r="O32" s="24">
         <f t="shared" si="10"/>
-        <v>23040</v>
+        <v>31294080</v>
       </c>
       <c r="P32" s="24">
         <f t="shared" ref="P32:Q32" si="11">SUM(P25:P31)</f>
-        <v>10032</v>
+        <v>15355040</v>
       </c>
       <c r="Q32" s="24">
         <f t="shared" si="11"/>
-        <v>7480.0000000000009</v>
+        <v>11079200</v>
       </c>
       <c r="R32" s="24">
         <f>SUM(R25:R31)</f>
-        <v>11160</v>
+        <v>15875760</v>
       </c>
       <c r="S32" s="24">
         <f>SUM(S25:S31)</f>
-        <v>60352</v>
+        <v>88628800</v>
       </c>
       <c r="T32" s="25">
         <f t="shared" si="8"/>
-        <v>167639</v>
+        <v>260217653</v>
       </c>
     </row>
     <row r="33" spans="1:89" x14ac:dyDescent="0.45">
@@ -2027,7 +2034,7 @@
         <v>2017</v>
       </c>
       <c r="B33" s="7">
-        <v>25</v>
+        <v>43204</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>17</v>
@@ -2038,21 +2045,21 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5">
         <f>$M6 * (B33*B11)</f>
-        <v>1500</v>
+        <v>2592240</v>
       </c>
       <c r="I33" s="24">
         <f t="shared" si="2"/>
-        <v>1500</v>
+        <v>2592240</v>
       </c>
       <c r="J33" s="5">
         <f>$D6 * (B33*B12)</f>
-        <v>1000</v>
+        <v>1728160</v>
       </c>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="24">
         <f t="shared" si="6"/>
-        <v>1000</v>
+        <v>1728160</v>
       </c>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
@@ -2060,83 +2067,83 @@
       <c r="Q33" s="5"/>
       <c r="R33" s="5">
         <f>$H6 * (B33*B13)</f>
-        <v>3000</v>
+        <v>5184480.0000000009</v>
       </c>
       <c r="S33" s="24">
         <f t="shared" si="7"/>
-        <v>3000</v>
+        <v>5184480.0000000009</v>
       </c>
       <c r="T33" s="25">
         <f t="shared" si="8"/>
-        <v>5500</v>
+        <v>9504880</v>
       </c>
     </row>
     <row r="34" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A34" s="17"/>
       <c r="B34" s="7">
-        <v>15</v>
+        <v>37463</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D34" s="5">
         <f>$B6 * (B34*B11)</f>
-        <v>10800</v>
+        <v>26973360</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5">
         <f>$L6 * (B34*B11)</f>
-        <v>1800</v>
+        <v>4495560</v>
       </c>
       <c r="H34" s="5">
         <f>$M6*(B34*B11)</f>
-        <v>900</v>
+        <v>2247780</v>
       </c>
       <c r="I34" s="24">
         <f t="shared" si="2"/>
-        <v>13500</v>
+        <v>33716700</v>
       </c>
       <c r="J34" s="5">
         <f>$D6 * (B34*B12)</f>
-        <v>600</v>
+        <v>1498520</v>
       </c>
       <c r="K34" s="5">
         <f>$I6 * (B34*B12)</f>
-        <v>6000</v>
+        <v>14985200</v>
       </c>
       <c r="L34" s="5"/>
       <c r="M34" s="24">
         <f t="shared" si="6"/>
-        <v>6600</v>
+        <v>16483720</v>
       </c>
       <c r="N34" s="5">
         <f>$A6 * (B34*B13)</f>
-        <v>3600</v>
+        <v>8991120</v>
       </c>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
       <c r="Q34" s="5">
         <f>$G6 * (B34*B13)</f>
-        <v>6600</v>
+        <v>16483720</v>
       </c>
       <c r="R34" s="5">
         <f>$H6 * (B34*B13)</f>
-        <v>1800</v>
+        <v>4495560</v>
       </c>
       <c r="S34" s="24">
         <f t="shared" si="7"/>
-        <v>12000</v>
+        <v>29970400</v>
       </c>
       <c r="T34" s="25">
         <f t="shared" si="8"/>
-        <v>32100</v>
+        <v>80170820</v>
       </c>
     </row>
     <row r="35" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A35" s="17"/>
       <c r="B35" s="7">
-        <v>17</v>
+        <v>34774</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>19</v>
@@ -2144,117 +2151,117 @@
       <c r="D35" s="5"/>
       <c r="E35" s="5">
         <f>$C6 * (B35*B11)</f>
-        <v>2039.9999999999998</v>
+        <v>4172879.9999999995</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5">
         <f>$M6 * (B35*B11)</f>
-        <v>1019.9999999999999</v>
+        <v>2086439.9999999998</v>
       </c>
       <c r="I35" s="24">
         <f t="shared" si="2"/>
-        <v>3059.9999999999995</v>
+        <v>6259319.9999999991</v>
       </c>
       <c r="J35" s="5">
         <f>$D6 * (B35*B12)</f>
-        <v>680</v>
+        <v>1390960</v>
       </c>
       <c r="K35" s="5"/>
       <c r="L35" s="5">
         <f>$J6 * (B35*B12)</f>
-        <v>2295</v>
+        <v>4694490</v>
       </c>
       <c r="M35" s="24">
         <f t="shared" si="6"/>
-        <v>2975</v>
+        <v>6085450</v>
       </c>
       <c r="N35" s="5">
         <f>$A6 * (B35*B13)</f>
-        <v>4080.0000000000005</v>
+        <v>8345760</v>
       </c>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
       <c r="R35" s="5">
         <f>$H6 * (B35*B13)</f>
-        <v>2040.0000000000002</v>
+        <v>4172880</v>
       </c>
       <c r="S35" s="24">
         <f t="shared" si="7"/>
-        <v>6120.0000000000009</v>
+        <v>12518640</v>
       </c>
       <c r="T35" s="25">
         <f t="shared" si="8"/>
-        <v>12155</v>
+        <v>24863410</v>
       </c>
     </row>
     <row r="36" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A36" s="17"/>
       <c r="B36" s="7">
-        <v>20</v>
+        <v>22597</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="5">
         <f>$B6 * (B36*B11)</f>
-        <v>14400</v>
+        <v>16269839.999999998</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5">
         <f>$K6 * (B36*B11)</f>
-        <v>5280</v>
+        <v>5965607.9999999991</v>
       </c>
       <c r="G36" s="5">
         <f>$L6 * (B36*B11)</f>
-        <v>2400</v>
+        <v>2711640</v>
       </c>
       <c r="H36" s="5">
         <f>$M6 * (B36*B11)</f>
-        <v>1200</v>
+        <v>1355820</v>
       </c>
       <c r="I36" s="24">
         <f t="shared" si="2"/>
-        <v>23280</v>
+        <v>26302907.999999996</v>
       </c>
       <c r="J36" s="5">
         <f>$D6 * (B36*B12)</f>
-        <v>800</v>
+        <v>903880</v>
       </c>
       <c r="K36" s="5">
         <f>$I6 * (B36*B12)</f>
-        <v>8000</v>
+        <v>9038800</v>
       </c>
       <c r="L36" s="5"/>
       <c r="M36" s="24">
         <f t="shared" si="6"/>
-        <v>8800</v>
+        <v>9942680</v>
       </c>
       <c r="N36" s="5"/>
       <c r="O36" s="5">
         <f>$E6 * (B36*B13)</f>
-        <v>7200</v>
+        <v>8134920.0000000009</v>
       </c>
       <c r="P36" s="5">
         <f>$F6 * (B36*B13)</f>
-        <v>6080</v>
+        <v>6869488.0000000009</v>
       </c>
       <c r="Q36" s="5"/>
       <c r="R36" s="5"/>
       <c r="S36" s="24">
         <f t="shared" si="7"/>
-        <v>13280</v>
+        <v>15004408.000000002</v>
       </c>
       <c r="T36" s="25">
         <f t="shared" si="8"/>
-        <v>45360</v>
+        <v>51249996</v>
       </c>
     </row>
     <row r="37" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A37" s="17"/>
       <c r="B37" s="7">
-        <v>18</v>
+        <v>24520</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>21</v>
@@ -2262,108 +2269,108 @@
       <c r="D37" s="5"/>
       <c r="E37" s="5">
         <f>$C6 * (B37*B11)</f>
-        <v>2160</v>
+        <v>2942400</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5">
         <f>$M6 * (B37*B11)</f>
-        <v>1080</v>
+        <v>1471200</v>
       </c>
       <c r="I37" s="24">
         <f t="shared" si="2"/>
-        <v>3240</v>
+        <v>4413600</v>
       </c>
       <c r="J37" s="5"/>
       <c r="K37" s="5">
         <f>$I6 * (B37*B12)</f>
-        <v>7200</v>
+        <v>9808000</v>
       </c>
       <c r="L37" s="5"/>
       <c r="M37" s="24">
         <f t="shared" si="6"/>
-        <v>7200</v>
+        <v>9808000</v>
       </c>
       <c r="N37" s="5"/>
       <c r="O37" s="5">
         <f>$E6 * (B37*B13)</f>
-        <v>6480</v>
+        <v>8827200</v>
       </c>
       <c r="P37" s="5"/>
       <c r="Q37" s="5">
         <f>$G6 * (B37*B13)</f>
-        <v>7920</v>
+        <v>10788800</v>
       </c>
       <c r="R37" s="5"/>
       <c r="S37" s="24">
         <f t="shared" si="7"/>
-        <v>14400</v>
+        <v>19616000</v>
       </c>
       <c r="T37" s="25">
         <f t="shared" si="8"/>
-        <v>24840</v>
+        <v>33837600</v>
       </c>
     </row>
     <row r="38" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A38" s="17"/>
       <c r="B38" s="7">
-        <v>17</v>
+        <v>23581</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D38" s="5">
         <f>$B6 * (B38*B11)</f>
-        <v>12240</v>
+        <v>16978320</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5">
         <f>$L6 * (B38*B11)</f>
-        <v>2039.9999999999998</v>
+        <v>2829720</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="24">
         <f t="shared" si="2"/>
-        <v>14280</v>
+        <v>19808040</v>
       </c>
       <c r="J38" s="5">
         <f>$D6 * (B38*B12)</f>
-        <v>680</v>
+        <v>943240</v>
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="5">
         <f>$J6 * (B38*B12)</f>
-        <v>2295</v>
+        <v>3183435</v>
       </c>
       <c r="M38" s="24">
         <f t="shared" si="6"/>
-        <v>2975</v>
+        <v>4126675</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5">
         <f>$F6 * (B28*B13)</f>
-        <v>6384</v>
+        <v>7069216</v>
       </c>
       <c r="Q38" s="5"/>
       <c r="R38" s="5">
         <f>$H6 * (B38*B13)</f>
-        <v>2040.0000000000002</v>
+        <v>2829720</v>
       </c>
       <c r="S38" s="24">
         <f t="shared" si="7"/>
-        <v>8424</v>
+        <v>9898936</v>
       </c>
       <c r="T38" s="25">
         <f t="shared" si="8"/>
-        <v>25679</v>
+        <v>33833651</v>
       </c>
     </row>
     <row r="39" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A39" s="17"/>
       <c r="B39" s="7">
-        <v>14</v>
+        <v>26077</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>23</v>
@@ -2372,45 +2379,45 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5">
         <f>$K6 * (B39*B11)</f>
-        <v>3696</v>
+        <v>6884327.9999999991</v>
       </c>
       <c r="G39" s="5"/>
       <c r="H39" s="5">
         <f>$M6 * (B39*B11)</f>
-        <v>840</v>
+        <v>1564620</v>
       </c>
       <c r="I39" s="24">
         <f t="shared" si="2"/>
-        <v>4536</v>
+        <v>8448948</v>
       </c>
       <c r="J39" s="5">
         <f>$D6 * (B39*B12)</f>
-        <v>560</v>
+        <v>1043080</v>
       </c>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
       <c r="M39" s="24">
         <f t="shared" si="6"/>
-        <v>560</v>
+        <v>1043080</v>
       </c>
       <c r="N39" s="5">
         <f>$A6 * (B39*B13)</f>
-        <v>3360.0000000000005</v>
+        <v>6258480.0000000009</v>
       </c>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
       <c r="R39" s="5">
         <f>$H6 * (B39*B13)</f>
-        <v>1680.0000000000002</v>
+        <v>3129240.0000000005</v>
       </c>
       <c r="S39" s="24">
         <f t="shared" si="7"/>
-        <v>5040.0000000000009</v>
+        <v>9387720.0000000019</v>
       </c>
       <c r="T39" s="25">
         <f t="shared" si="8"/>
-        <v>10136</v>
+        <v>18879748</v>
       </c>
     </row>
     <row r="40" spans="1:89" x14ac:dyDescent="0.45">
@@ -2418,76 +2425,77 @@
         <v>31</v>
       </c>
       <c r="B40" s="31">
-        <v>224547</v>
+        <f>SUM(B33:B39)</f>
+        <v>212216</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="24">
         <f t="shared" ref="D40:S40" si="12">SUM(D33:D39)</f>
-        <v>37440</v>
+        <v>60221520</v>
       </c>
       <c r="E40" s="24">
         <f t="shared" si="12"/>
-        <v>4200</v>
+        <v>7115280</v>
       </c>
       <c r="F40" s="24">
         <f t="shared" si="12"/>
-        <v>8976</v>
+        <v>12849935.999999998</v>
       </c>
       <c r="G40" s="24">
         <f t="shared" si="12"/>
-        <v>6240</v>
+        <v>10036920</v>
       </c>
       <c r="H40" s="24">
         <f>SUM(H33:H39)</f>
-        <v>6540</v>
+        <v>11318100</v>
       </c>
       <c r="I40" s="24">
         <f t="shared" si="12"/>
-        <v>63396</v>
+        <v>101541756</v>
       </c>
       <c r="J40" s="24">
         <f t="shared" si="12"/>
-        <v>4320</v>
+        <v>7507840</v>
       </c>
       <c r="K40" s="24">
         <f t="shared" si="12"/>
-        <v>21200</v>
+        <v>33832000</v>
       </c>
       <c r="L40" s="24">
         <f t="shared" si="12"/>
-        <v>4590</v>
+        <v>7877925</v>
       </c>
       <c r="M40" s="24">
         <f t="shared" si="12"/>
-        <v>30110</v>
+        <v>49217765</v>
       </c>
       <c r="N40" s="24">
         <f t="shared" si="12"/>
-        <v>11040</v>
+        <v>23595360</v>
       </c>
       <c r="O40" s="24">
         <f t="shared" si="12"/>
-        <v>13680</v>
+        <v>16962120</v>
       </c>
       <c r="P40" s="24">
         <f t="shared" si="12"/>
-        <v>12464</v>
+        <v>13938704</v>
       </c>
       <c r="Q40" s="24">
         <f t="shared" si="12"/>
-        <v>14520</v>
+        <v>27272520</v>
       </c>
       <c r="R40" s="24">
         <f t="shared" si="12"/>
-        <v>10560</v>
+        <v>19811880</v>
       </c>
       <c r="S40" s="24">
         <f t="shared" si="12"/>
-        <v>62264</v>
+        <v>101580584</v>
       </c>
       <c r="T40" s="25">
         <f t="shared" si="8"/>
-        <v>155770</v>
+        <v>252340105</v>
       </c>
     </row>
     <row r="41" spans="1:89" x14ac:dyDescent="0.45">
@@ -2495,7 +2503,7 @@
         <v>2016</v>
       </c>
       <c r="B41" s="7">
-        <v>27</v>
+        <v>42350</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>17</v>
@@ -2506,21 +2514,21 @@
       <c r="G41" s="5"/>
       <c r="H41" s="5">
         <f>$M6 * (B41*B11)</f>
-        <v>1620</v>
+        <v>2541000</v>
       </c>
       <c r="I41" s="24">
         <f>SUM(D41:H41)</f>
-        <v>1620</v>
+        <v>2541000</v>
       </c>
       <c r="J41" s="5">
         <f>$D6 * (B41*B12)</f>
-        <v>1080</v>
+        <v>1694000</v>
       </c>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
       <c r="M41" s="24">
         <f>SUM(J41:L41)</f>
-        <v>1080</v>
+        <v>1694000</v>
       </c>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
@@ -2528,21 +2536,21 @@
       <c r="Q41" s="5"/>
       <c r="R41" s="5">
         <f>$H6 * (B41*B13)</f>
-        <v>3240</v>
+        <v>5082000</v>
       </c>
       <c r="S41" s="24">
         <f>SUM(N41:R41)</f>
-        <v>3240</v>
+        <v>5082000</v>
       </c>
       <c r="T41" s="25">
         <f>SUM(I41+M41+S41)</f>
-        <v>5940</v>
+        <v>9317000</v>
       </c>
     </row>
     <row r="42" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A42" s="17"/>
       <c r="B42" s="7">
-        <v>25</v>
+        <v>36189</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>18</v>
@@ -2551,45 +2559,45 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5">
         <f>$K6 * (B42*B11)</f>
-        <v>6600</v>
+        <v>9553895.9999999981</v>
       </c>
       <c r="G42" s="5"/>
       <c r="H42" s="5">
         <f>$M6 * (B42*B11)</f>
-        <v>1500</v>
+        <v>2171340</v>
       </c>
       <c r="I42" s="24">
         <f t="shared" ref="I42:I47" si="13">SUM(D42:H42)</f>
-        <v>8100</v>
+        <v>11725235.999999998</v>
       </c>
       <c r="J42" s="5">
         <f>$D6 * (B42*B12)</f>
-        <v>1000</v>
+        <v>1447560</v>
       </c>
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
       <c r="M42" s="24">
         <f t="shared" ref="M42:M47" si="14">SUM(J42:L42)</f>
-        <v>1000</v>
+        <v>1447560</v>
       </c>
       <c r="N42" s="5"/>
       <c r="O42" s="5">
         <f>$E6 * (B42*B13)</f>
-        <v>9000</v>
+        <v>13028040</v>
       </c>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
       <c r="R42" s="5">
         <f>$H6 * (B42*B13)</f>
-        <v>3000</v>
+        <v>4342680</v>
       </c>
       <c r="S42" s="24">
         <f t="shared" ref="S42:S47" si="15">SUM(N42:R42)</f>
-        <v>12000</v>
+        <v>17370720</v>
       </c>
       <c r="T42" s="25">
         <f t="shared" ref="T42:T47" si="16">SUM(I42+M42+S42)</f>
-        <v>21100</v>
+        <v>30543516</v>
       </c>
       <c r="Y42" s="20"/>
       <c r="Z42" s="20"/>
@@ -2660,60 +2668,60 @@
     <row r="43" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A43" s="17"/>
       <c r="B43" s="1">
-        <v>19</v>
+        <v>33508</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D43" s="5">
         <f>$B6 * (B43*B11)</f>
-        <v>13680</v>
+        <v>24125760</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5">
         <f>$M6 * (B43*B11)</f>
-        <v>1140</v>
+        <v>2010480</v>
       </c>
       <c r="I43" s="24">
         <f t="shared" si="13"/>
-        <v>14820</v>
+        <v>26136240</v>
       </c>
       <c r="J43" s="5">
         <f>$D6 * (B43*B12)</f>
-        <v>760</v>
+        <v>1340320</v>
       </c>
       <c r="K43" s="5"/>
       <c r="L43" s="5">
         <f>$J6 * (B43*B12)</f>
-        <v>2565</v>
+        <v>4523580</v>
       </c>
       <c r="M43" s="24">
         <f t="shared" si="14"/>
-        <v>3325</v>
+        <v>5863900</v>
       </c>
       <c r="N43" s="5"/>
       <c r="O43" s="5">
         <f>$E6 * (B43*B13)</f>
-        <v>6840.0000000000009</v>
+        <v>12062880</v>
       </c>
       <c r="P43" s="5"/>
       <c r="Q43" s="5">
         <f>$G6 * (B43*B13)</f>
-        <v>8360</v>
+        <v>14743520</v>
       </c>
       <c r="R43" s="5">
         <f>$H6 * (B43*B13)</f>
-        <v>2280</v>
+        <v>4020960</v>
       </c>
       <c r="S43" s="24">
         <f t="shared" si="15"/>
-        <v>17480</v>
+        <v>30827360</v>
       </c>
       <c r="T43" s="25">
         <f t="shared" si="16"/>
-        <v>35625</v>
+        <v>62827500</v>
       </c>
       <c r="Y43" s="20"/>
       <c r="Z43" s="20"/>
@@ -2784,7 +2792,7 @@
     <row r="44" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A44" s="17"/>
       <c r="B44" s="1">
-        <v>20</v>
+        <v>21644</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>20</v>
@@ -2792,49 +2800,49 @@
       <c r="D44" s="5"/>
       <c r="E44" s="5">
         <f>$C6 * (B44*B11)</f>
-        <v>2400</v>
+        <v>2597280</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5">
         <f>$L6 * (B44*B11)</f>
-        <v>2400</v>
+        <v>2597280</v>
       </c>
       <c r="H44" s="5">
         <f>$M6 * (B44*B11)</f>
-        <v>1200</v>
+        <v>1298640</v>
       </c>
       <c r="I44" s="24">
         <f t="shared" si="13"/>
-        <v>6000</v>
+        <v>6493200</v>
       </c>
       <c r="J44" s="5">
         <f>$D6 * (B44*B12)</f>
-        <v>800</v>
+        <v>865760</v>
       </c>
       <c r="K44" s="5">
         <f>$I6 * (B44*B12)</f>
-        <v>8000</v>
+        <v>8657600</v>
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="24">
         <f t="shared" si="14"/>
-        <v>8800</v>
+        <v>9523360</v>
       </c>
       <c r="N44" s="5"/>
       <c r="O44" s="5">
         <f>$E6 * (B44*B13)</f>
-        <v>7200</v>
+        <v>7791840</v>
       </c>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
       <c r="S44" s="24">
         <f t="shared" si="15"/>
-        <v>7200</v>
+        <v>7791840</v>
       </c>
       <c r="T44" s="25">
         <f t="shared" si="16"/>
-        <v>22000</v>
+        <v>23808400</v>
       </c>
       <c r="Y44" s="20"/>
       <c r="Z44" s="20"/>
@@ -2905,7 +2913,7 @@
     <row r="45" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A45" s="17"/>
       <c r="B45" s="1">
-        <v>18</v>
+        <v>22911</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>21</v>
@@ -2913,46 +2921,46 @@
       <c r="D45" s="5"/>
       <c r="E45" s="5">
         <f>$C6 * (B45*B11)</f>
-        <v>2160</v>
+        <v>2749320</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5">
         <f>$M6 * (B45*B11)</f>
-        <v>1080</v>
+        <v>1374660</v>
       </c>
       <c r="I45" s="24">
         <f>SUM(D45:H45)</f>
-        <v>3240</v>
+        <v>4123980</v>
       </c>
       <c r="J45" s="5">
         <f>$D6 * (B45*B12)</f>
-        <v>720</v>
+        <v>916440</v>
       </c>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
       <c r="M45" s="24">
         <f>SUM(J45:L45)</f>
-        <v>720</v>
+        <v>916440</v>
       </c>
       <c r="N45" s="5">
         <f>$A6 * (B45*B13)</f>
-        <v>4320</v>
+        <v>5498640</v>
       </c>
       <c r="O45" s="5"/>
       <c r="P45" s="5">
         <f>$F6 * (B45*B13)</f>
-        <v>5472</v>
+        <v>6964944</v>
       </c>
       <c r="Q45" s="5"/>
       <c r="R45" s="5"/>
       <c r="S45" s="24">
         <f>SUM(N45:R45)</f>
-        <v>9792</v>
+        <v>12463584</v>
       </c>
       <c r="T45" s="25">
         <f t="shared" si="16"/>
-        <v>13752</v>
+        <v>17504004</v>
       </c>
       <c r="Y45" s="20"/>
       <c r="Z45" s="20"/>
@@ -3023,54 +3031,54 @@
     <row r="46" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A46" s="17"/>
       <c r="B46" s="1">
-        <v>21</v>
+        <v>24191</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D46" s="5">
         <f>$B6 * (B46*B11)</f>
-        <v>15120</v>
+        <v>17417520</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5">
         <f>$M6 * (B46*B11)</f>
-        <v>1260</v>
+        <v>1451460</v>
       </c>
       <c r="I46" s="24">
         <f t="shared" si="13"/>
-        <v>16380</v>
+        <v>18868980</v>
       </c>
       <c r="J46" s="5">
         <f>$D6 * (B46*B12)</f>
-        <v>840</v>
+        <v>967640</v>
       </c>
       <c r="K46" s="5">
         <f>$I6 * (B46*B12)</f>
-        <v>8400</v>
+        <v>9676400</v>
       </c>
       <c r="L46" s="5"/>
       <c r="M46" s="24">
         <f t="shared" si="14"/>
-        <v>9240</v>
+        <v>10644040</v>
       </c>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
       <c r="Q46" s="5">
         <f>$G6 * (B46*B13)</f>
-        <v>9240</v>
+        <v>10644040</v>
       </c>
       <c r="R46" s="5"/>
       <c r="S46" s="24">
         <f t="shared" si="15"/>
-        <v>9240</v>
+        <v>10644040</v>
       </c>
       <c r="T46" s="25">
         <f t="shared" si="16"/>
-        <v>34860</v>
+        <v>40157060</v>
       </c>
       <c r="Y46" s="20"/>
       <c r="Z46" s="20"/>
@@ -3141,7 +3149,7 @@
     <row r="47" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A47" s="17"/>
       <c r="B47" s="1">
-        <v>24</v>
+        <v>25412</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>23</v>
@@ -3152,40 +3160,40 @@
       <c r="G47" s="5"/>
       <c r="H47" s="5">
         <f>$M6 * (B47*B11)</f>
-        <v>1439.9999999999998</v>
+        <v>1524720</v>
       </c>
       <c r="I47" s="24">
         <f t="shared" si="13"/>
-        <v>1439.9999999999998</v>
+        <v>1524720</v>
       </c>
       <c r="J47" s="5">
         <f>$D6 * (B47*B12)</f>
-        <v>960</v>
+        <v>1016480</v>
       </c>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
       <c r="M47" s="24">
         <f t="shared" si="14"/>
-        <v>960</v>
+        <v>1016480</v>
       </c>
       <c r="N47" s="5"/>
       <c r="O47" s="5">
         <f>$E6 * (B47*B13)</f>
-        <v>8640.0000000000018</v>
+        <v>9148320.0000000019</v>
       </c>
       <c r="P47" s="5"/>
       <c r="Q47" s="5"/>
       <c r="R47" s="5">
         <f>$H6 * (B47*B13)</f>
-        <v>2880.0000000000005</v>
+        <v>3049440.0000000005</v>
       </c>
       <c r="S47" s="24">
         <f t="shared" si="15"/>
-        <v>11520.000000000002</v>
+        <v>12197760.000000002</v>
       </c>
       <c r="T47" s="25">
         <f t="shared" si="16"/>
-        <v>13920.000000000002</v>
+        <v>14738960.000000002</v>
       </c>
       <c r="U47" s="20"/>
       <c r="V47" s="20"/>
@@ -3260,75 +3268,76 @@
     <row r="48" spans="1:89" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A48" s="18"/>
       <c r="B48" s="31">
-        <v>217792</v>
+        <f>SUM(B41:B47)</f>
+        <v>206205</v>
       </c>
       <c r="D48" s="24">
         <f t="shared" ref="D48:N48" si="17">SUM(D41:D47)</f>
-        <v>28800</v>
+        <v>41543280</v>
       </c>
       <c r="E48" s="24">
         <f t="shared" si="17"/>
-        <v>4560</v>
+        <v>5346600</v>
       </c>
       <c r="F48" s="24">
         <f t="shared" si="17"/>
-        <v>6600</v>
+        <v>9553895.9999999981</v>
       </c>
       <c r="G48" s="24">
         <f t="shared" si="17"/>
-        <v>2400</v>
+        <v>2597280</v>
       </c>
       <c r="H48" s="24">
         <f t="shared" si="17"/>
-        <v>9240</v>
+        <v>12372300</v>
       </c>
       <c r="I48" s="24">
         <f t="shared" si="17"/>
-        <v>51600</v>
+        <v>71413356</v>
       </c>
       <c r="J48" s="24">
         <f t="shared" si="17"/>
-        <v>6160</v>
+        <v>8248200</v>
       </c>
       <c r="K48" s="24">
         <f t="shared" si="17"/>
-        <v>16400</v>
+        <v>18334000</v>
       </c>
       <c r="L48" s="24">
         <f t="shared" si="17"/>
-        <v>2565</v>
+        <v>4523580</v>
       </c>
       <c r="M48" s="24">
         <f t="shared" si="17"/>
-        <v>25125</v>
+        <v>31105780</v>
       </c>
       <c r="N48" s="24">
         <f t="shared" si="17"/>
-        <v>4320</v>
+        <v>5498640</v>
       </c>
       <c r="O48" s="24">
         <f t="shared" ref="O48:R48" si="18">SUM(O41:O47)</f>
-        <v>31680</v>
+        <v>42031080</v>
       </c>
       <c r="P48" s="24">
         <f>SUM(P41:P47)</f>
-        <v>5472</v>
+        <v>6964944</v>
       </c>
       <c r="Q48" s="24">
         <f t="shared" si="18"/>
-        <v>17600</v>
+        <v>25387560</v>
       </c>
       <c r="R48" s="24">
         <f t="shared" si="18"/>
-        <v>11400</v>
+        <v>16495080</v>
       </c>
       <c r="S48" s="24">
         <f>SUM(S41:S47)</f>
-        <v>70472</v>
+        <v>96377304</v>
       </c>
       <c r="T48" s="25">
         <f>SUM(T41:T47)</f>
-        <v>147197</v>
+        <v>198896440</v>
       </c>
       <c r="U48" s="20"/>
       <c r="V48" s="20"/>
@@ -3405,7 +3414,7 @@
         <v>2015</v>
       </c>
       <c r="B49" s="1">
-        <v>24</v>
+        <v>40453</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>17</v>
@@ -3416,37 +3425,37 @@
       <c r="G49" s="5"/>
       <c r="H49" s="5">
         <f>$M6 * (B49*B11)</f>
-        <v>1439.9999999999998</v>
+        <v>2427180</v>
       </c>
       <c r="I49" s="24">
         <f t="shared" ref="I49:I55" si="19">SUM(D49:H49)</f>
-        <v>1439.9999999999998</v>
+        <v>2427180</v>
       </c>
       <c r="J49" s="5">
         <f>$D6 * (B49*B12)</f>
-        <v>960</v>
+        <v>1618120</v>
       </c>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
       <c r="M49" s="24">
         <f>SUM(J49:L49)</f>
-        <v>960</v>
+        <v>1618120</v>
       </c>
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
       <c r="P49" s="5">
         <f>$F6 * (B49*B13)</f>
-        <v>7296.0000000000009</v>
+        <v>12297712</v>
       </c>
       <c r="Q49" s="5"/>
       <c r="R49" s="5"/>
       <c r="S49" s="24">
         <f>SUM(N49:R49)</f>
-        <v>7296.0000000000009</v>
+        <v>12297712</v>
       </c>
       <c r="T49" s="25">
         <f>SUM(I49+M49+S49)</f>
-        <v>9696</v>
+        <v>16343012</v>
       </c>
       <c r="U49" s="20"/>
       <c r="V49" s="20"/>
@@ -3521,7 +3530,7 @@
     <row r="50" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A50" s="1"/>
       <c r="B50" s="1">
-        <v>21</v>
+        <v>34008</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>18</v>
@@ -3532,46 +3541,46 @@
       <c r="G50" s="5"/>
       <c r="H50" s="5">
         <f>$M6 * (B50*B11)</f>
-        <v>1260</v>
+        <v>2040480</v>
       </c>
       <c r="I50" s="24">
         <f t="shared" si="19"/>
-        <v>1260</v>
+        <v>2040480</v>
       </c>
       <c r="J50" s="5">
         <f>$D6 * (B50*B12)</f>
-        <v>840</v>
+        <v>1360320</v>
       </c>
       <c r="K50" s="5">
         <f>$I6 * (B50*B12)</f>
-        <v>8400</v>
+        <v>13603200</v>
       </c>
       <c r="L50" s="5"/>
       <c r="M50" s="24">
         <f t="shared" ref="M50:M55" si="20">SUM(J50:L50)</f>
-        <v>9240</v>
+        <v>14963520</v>
       </c>
       <c r="N50" s="5"/>
       <c r="O50" s="5">
         <f>$E6 * (B50*B13)</f>
-        <v>7560</v>
+        <v>12242880</v>
       </c>
       <c r="P50" s="5">
         <f>$F6 * (B50*B13)</f>
-        <v>6384</v>
+        <v>10338432</v>
       </c>
       <c r="Q50" s="5"/>
       <c r="R50" s="5">
         <f>$J6 * (B50*B12)</f>
-        <v>2835</v>
+        <v>4591080</v>
       </c>
       <c r="S50" s="24">
         <f t="shared" ref="S50:S55" si="21">SUM(N50:R50)</f>
-        <v>16779</v>
+        <v>27172392</v>
       </c>
       <c r="T50" s="25">
         <f t="shared" ref="T50:T55" si="22">SUM(I50+M50+S50)</f>
-        <v>27279</v>
+        <v>44176392</v>
       </c>
       <c r="U50" s="20"/>
       <c r="V50" s="20"/>
@@ -3646,57 +3655,57 @@
     <row r="51" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A51" s="1"/>
       <c r="B51" s="1">
-        <v>19</v>
+        <v>31395</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D51" s="5">
         <f>$L6 * (B51*B11)</f>
-        <v>2280</v>
+        <v>3767400</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
       <c r="G51" s="5">
         <f>$L6 * (B51*B11)</f>
-        <v>2280</v>
+        <v>3767400</v>
       </c>
       <c r="H51" s="5">
         <f>$M6 * (B51*B11)</f>
-        <v>1140</v>
+        <v>1883700</v>
       </c>
       <c r="I51" s="24">
         <f t="shared" si="19"/>
-        <v>5700</v>
+        <v>9418500</v>
       </c>
       <c r="J51" s="5">
         <f>$D6 * (B51*B12)</f>
-        <v>760</v>
+        <v>1255800</v>
       </c>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
       <c r="M51" s="24">
         <f t="shared" si="20"/>
-        <v>760</v>
+        <v>1255800</v>
       </c>
       <c r="N51" s="5">
         <f>$A6 * (B51*B13)</f>
-        <v>4560</v>
+        <v>7534800</v>
       </c>
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
       <c r="Q51" s="5">
         <f>$G6 * (B51*B13)</f>
-        <v>8360</v>
+        <v>13813800</v>
       </c>
       <c r="R51" s="5"/>
       <c r="S51" s="24">
         <f t="shared" si="21"/>
-        <v>12920</v>
+        <v>21348600</v>
       </c>
       <c r="T51" s="25">
         <f t="shared" si="22"/>
-        <v>19380</v>
+        <v>32022900</v>
       </c>
       <c r="U51" s="20"/>
       <c r="V51" s="20"/>
@@ -3771,7 +3780,7 @@
     <row r="52" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A52" s="1"/>
       <c r="B52" s="1">
-        <v>18</v>
+        <v>21069</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>20</v>
@@ -3779,52 +3788,52 @@
       <c r="D52" s="5"/>
       <c r="E52" s="5">
         <f>$C6 * (B52*B11)</f>
-        <v>2160</v>
+        <v>2528280</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5">
         <f>$L6 * (B52*B11)</f>
-        <v>2160</v>
+        <v>2528280</v>
       </c>
       <c r="H52" s="5">
         <f>$M6 * (B52*B11)</f>
-        <v>1080</v>
+        <v>1264140</v>
       </c>
       <c r="I52" s="24">
         <f t="shared" si="19"/>
-        <v>5400</v>
+        <v>6320700</v>
       </c>
       <c r="J52" s="5">
         <f>$D6 * (B52*B12)</f>
-        <v>720</v>
+        <v>842760</v>
       </c>
       <c r="K52" s="5"/>
       <c r="L52" s="5">
         <f>$J6 * (B52*B12)</f>
-        <v>2430</v>
+        <v>2844315</v>
       </c>
       <c r="M52" s="24">
         <f t="shared" si="20"/>
-        <v>3150</v>
+        <v>3687075</v>
       </c>
       <c r="N52" s="5"/>
       <c r="O52" s="5">
         <f>$E6 * (B52*B13)</f>
-        <v>6480</v>
+        <v>7584840</v>
       </c>
       <c r="P52" s="5"/>
       <c r="Q52" s="5">
         <f>$G6 * (B52*B13)</f>
-        <v>7920</v>
+        <v>9270360</v>
       </c>
       <c r="R52" s="5"/>
       <c r="S52" s="24">
         <f t="shared" si="21"/>
-        <v>14400</v>
+        <v>16855200</v>
       </c>
       <c r="T52" s="25">
         <f t="shared" si="22"/>
-        <v>22950</v>
+        <v>26862975</v>
       </c>
       <c r="U52" s="20"/>
       <c r="V52" s="20"/>
@@ -3899,7 +3908,7 @@
     <row r="53" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A53" s="17"/>
       <c r="B53" s="1">
-        <v>22</v>
+        <v>23049</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>21</v>
@@ -3908,29 +3917,29 @@
       <c r="E53" s="5"/>
       <c r="F53" s="5">
         <f>$C6 * (B53*B11)</f>
-        <v>2640</v>
+        <v>2765880</v>
       </c>
       <c r="G53" s="5"/>
       <c r="H53" s="5">
         <f>$M6 * (B53*B11)</f>
-        <v>1320</v>
+        <v>1382940</v>
       </c>
       <c r="I53" s="24">
         <f t="shared" si="19"/>
-        <v>3960</v>
+        <v>4148820</v>
       </c>
       <c r="J53" s="5">
         <f>$D6 * (B53*B12)</f>
-        <v>880</v>
+        <v>921960</v>
       </c>
       <c r="K53" s="5">
         <f>$I6 * (B53*B12)</f>
-        <v>8800</v>
+        <v>9219600</v>
       </c>
       <c r="L53" s="5"/>
       <c r="M53" s="24">
         <f t="shared" si="20"/>
-        <v>9680</v>
+        <v>10141560</v>
       </c>
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
@@ -3943,7 +3952,7 @@
       </c>
       <c r="T53" s="25">
         <f t="shared" si="22"/>
-        <v>13640</v>
+        <v>14290380</v>
       </c>
       <c r="U53" s="20"/>
       <c r="V53" s="20"/>
@@ -4018,63 +4027,63 @@
     <row r="54" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A54" s="17"/>
       <c r="B54" s="1">
-        <v>21</v>
+        <v>22879</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D54" s="5">
         <f>$L6 * (B54*B11)</f>
-        <v>2520</v>
+        <v>2745480</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5">
         <f>$C6 * (B54*B11)</f>
-        <v>2520</v>
+        <v>2745480</v>
       </c>
       <c r="G54" s="5"/>
       <c r="H54" s="5">
         <f>$M6 * (B54*B11)</f>
-        <v>1260</v>
+        <v>1372740</v>
       </c>
       <c r="I54" s="24">
         <f t="shared" si="19"/>
-        <v>6300</v>
+        <v>6863700</v>
       </c>
       <c r="J54" s="5">
         <f>$D6 * (B54*B12)</f>
-        <v>840</v>
+        <v>915160</v>
       </c>
       <c r="K54" s="5"/>
       <c r="L54" s="5">
         <f>$J6 * (B54*B12)</f>
-        <v>2835</v>
+        <v>3088665</v>
       </c>
       <c r="M54" s="24">
         <f t="shared" si="20"/>
-        <v>3675</v>
+        <v>4003825</v>
       </c>
       <c r="N54" s="5">
         <f>$A6 * (B54*B13)</f>
-        <v>5040</v>
+        <v>5490960</v>
       </c>
       <c r="O54" s="5"/>
       <c r="P54" s="5">
         <f>$F6 * (B54*B13)</f>
-        <v>6384</v>
+        <v>6955216</v>
       </c>
       <c r="Q54" s="5"/>
       <c r="R54" s="5">
         <f>$H6 * (B54*B13)</f>
-        <v>2520</v>
+        <v>2745480</v>
       </c>
       <c r="S54" s="24">
         <f t="shared" si="21"/>
-        <v>13944</v>
+        <v>15191656</v>
       </c>
       <c r="T54" s="25">
         <f t="shared" si="22"/>
-        <v>23919</v>
+        <v>26059181</v>
       </c>
       <c r="U54" s="20"/>
       <c r="V54" s="20"/>
@@ -4149,7 +4158,7 @@
     <row r="55" spans="1:89" x14ac:dyDescent="0.45">
       <c r="A55" s="17"/>
       <c r="B55" s="1">
-        <v>28</v>
+        <v>23515</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>23</v>
@@ -4157,43 +4166,43 @@
       <c r="D55" s="5"/>
       <c r="E55" s="5">
         <f>$C6 * (B55*B11)</f>
-        <v>3360</v>
+        <v>2821800</v>
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5">
         <f>$M6 * (B55*B11)</f>
-        <v>1680</v>
+        <v>1410900</v>
       </c>
       <c r="I55" s="24">
         <f t="shared" si="19"/>
-        <v>5040</v>
+        <v>4232700</v>
       </c>
       <c r="J55" s="5">
         <f>$D6 * (B55*B12)</f>
-        <v>1120</v>
+        <v>940600</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
       <c r="M55" s="24">
         <f t="shared" si="20"/>
-        <v>1120</v>
+        <v>940600</v>
       </c>
       <c r="N55" s="5"/>
       <c r="O55" s="5"/>
       <c r="P55" s="5">
         <f>$F6 * (B55*B13)</f>
-        <v>8512</v>
+        <v>7148560</v>
       </c>
       <c r="Q55" s="5"/>
       <c r="R55" s="5"/>
       <c r="S55" s="24">
         <f t="shared" si="21"/>
-        <v>8512</v>
+        <v>7148560</v>
       </c>
       <c r="T55" s="25">
         <f t="shared" si="22"/>
-        <v>14672</v>
+        <v>12321860</v>
       </c>
       <c r="U55" s="20"/>
       <c r="V55" s="20"/>
@@ -4268,75 +4277,76 @@
     <row r="56" spans="1:89" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A56" s="18"/>
       <c r="B56" s="32">
-        <v>209049</v>
+        <f>SUM(B49:B55)</f>
+        <v>196368</v>
       </c>
       <c r="D56" s="24">
         <f>SUM(D49:D55)</f>
-        <v>4800</v>
+        <v>6512880</v>
       </c>
       <c r="E56" s="24">
         <f t="shared" ref="E56:G56" si="23">SUM(E49:E55)</f>
-        <v>5520</v>
+        <v>5350080</v>
       </c>
       <c r="F56" s="24">
         <f t="shared" si="23"/>
-        <v>5160</v>
+        <v>5511360</v>
       </c>
       <c r="G56" s="24">
         <f t="shared" si="23"/>
-        <v>4440</v>
+        <v>6295680</v>
       </c>
       <c r="H56" s="24">
         <f t="shared" ref="H56:N56" si="24">SUM(H49:H55)</f>
-        <v>9180</v>
+        <v>11782080</v>
       </c>
       <c r="I56" s="24">
         <f t="shared" si="24"/>
-        <v>29100</v>
+        <v>35452080</v>
       </c>
       <c r="J56" s="24">
         <f t="shared" si="24"/>
-        <v>6120</v>
+        <v>7854720</v>
       </c>
       <c r="K56" s="24">
         <f t="shared" si="24"/>
-        <v>17200</v>
+        <v>22822800</v>
       </c>
       <c r="L56" s="24">
         <f t="shared" si="24"/>
-        <v>5265</v>
+        <v>5932980</v>
       </c>
       <c r="M56" s="24">
         <f t="shared" si="24"/>
-        <v>28585</v>
+        <v>36610500</v>
       </c>
       <c r="N56" s="24">
         <f t="shared" si="24"/>
-        <v>9600</v>
+        <v>13025760</v>
       </c>
       <c r="O56" s="24">
         <f t="shared" ref="O56:R56" si="25">SUM(O49:O55)</f>
-        <v>14040</v>
+        <v>19827720</v>
       </c>
       <c r="P56" s="24">
         <f t="shared" si="25"/>
-        <v>28576</v>
+        <v>36739920</v>
       </c>
       <c r="Q56" s="24">
         <f t="shared" si="25"/>
-        <v>16280</v>
+        <v>23084160</v>
       </c>
       <c r="R56" s="24">
         <f t="shared" si="25"/>
-        <v>5355</v>
+        <v>7336560</v>
       </c>
       <c r="S56" s="24">
         <f>SUM(S49:S55)</f>
-        <v>73851</v>
+        <v>100014120</v>
       </c>
       <c r="T56" s="25">
         <f>SUM(I56+M56+S56)</f>
-        <v>131536</v>
+        <v>172076700</v>
       </c>
       <c r="U56" s="20"/>
       <c r="V56" s="20"/>
@@ -4413,77 +4423,77 @@
         <v>10</v>
       </c>
       <c r="B57" s="6">
-        <f>B24+B32+B40</f>
-        <v>693284</v>
+        <f>B24+B32+B40+B48+B56</f>
+        <v>1058515</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="25">
         <f>SUM(D24+D32+D40+D48+D56)</f>
-        <v>117840</v>
+        <v>185403120</v>
       </c>
       <c r="E57" s="25">
         <f>SUM(E24+E32+E40+E48+E56)</f>
-        <v>29040</v>
+        <v>39594840</v>
       </c>
       <c r="F57" s="25">
         <f>SUM(F24+F32+F40+F48+F56)</f>
-        <v>35784</v>
+        <v>50545272</v>
       </c>
       <c r="G57" s="25">
         <f>SUM(G24+G32+G40+G48+G56)</f>
-        <v>22440</v>
+        <v>32157120</v>
       </c>
       <c r="H57" s="25">
         <f>SUM(H24+H32+H40+H48+H56)</f>
-        <v>37920</v>
+        <v>54539460</v>
       </c>
       <c r="I57" s="25">
         <f>SUM(I40+I32+I24+I48+I56)</f>
-        <v>243024</v>
+        <v>362239812</v>
       </c>
       <c r="J57" s="25">
         <f>J24+J32+J40+J48+J56</f>
-        <v>19800</v>
+        <v>29041560</v>
       </c>
       <c r="K57" s="25">
         <f>K24+K32+K40+K48+K56</f>
-        <v>144800</v>
+        <v>207873200</v>
       </c>
       <c r="L57" s="25">
         <f>L24+L32+L40+L48+L56</f>
-        <v>25110</v>
+        <v>36959625</v>
       </c>
       <c r="M57" s="25">
         <f>M24+M32+M40+M48+M56</f>
-        <v>189710</v>
+        <v>273874385</v>
       </c>
       <c r="N57" s="25">
         <f>SUM(N24+N32+N40+N48+N56)</f>
-        <v>44880</v>
+        <v>74200320</v>
       </c>
       <c r="O57" s="25">
         <f t="shared" ref="O57:R57" si="26">SUM(O24+O32+O40+O48+O56)</f>
-        <v>110520</v>
+        <v>151408800</v>
       </c>
       <c r="P57" s="25">
         <f t="shared" si="26"/>
-        <v>74480</v>
+        <v>100816128</v>
       </c>
       <c r="Q57" s="25">
         <f t="shared" si="26"/>
-        <v>74800</v>
+        <v>122429560</v>
       </c>
       <c r="R57" s="25">
         <f t="shared" si="26"/>
-        <v>46155</v>
+        <v>71235240</v>
       </c>
       <c r="S57" s="25">
         <f>SUM(S24+S32+S40+S48+S56)</f>
-        <v>350835</v>
+        <v>520090048</v>
       </c>
       <c r="T57" s="30">
         <f>SUM(T40+T32+T24+T48+T56)</f>
-        <v>699673</v>
+        <v>1022715005</v>
       </c>
       <c r="U57" s="20"/>
       <c r="V57" s="20"/>
@@ -4635,12 +4645,12 @@
     </row>
     <row r="60" spans="1:89" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:89" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:89" x14ac:dyDescent="0.45">

</xml_diff>